<commit_message>
add the ability to remove host
</commit_message>
<xml_diff>
--- a/database architecture.xlsx
+++ b/database architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artem\Documents\Nastie\Nastie_server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EB9E226-BB33-44E5-ACD8-E4D93FE3EAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D85C905-4B44-4F67-BC4E-6881668FD195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{119B1A81-14A3-4158-B054-44CDDA5B70FD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>token1</t>
   </si>
@@ -57,13 +57,25 @@
     <t>token (varchar)</t>
   </si>
   <si>
-    <t>user_id (integer)</t>
-  </si>
-  <si>
     <t>table: users</t>
   </si>
   <si>
     <t>table: tokens</t>
+  </si>
+  <si>
+    <t>table: hosts</t>
+  </si>
+  <si>
+    <t>name (varchar)</t>
+  </si>
+  <si>
+    <t>Изотова А.А.</t>
+  </si>
+  <si>
+    <t>user_id (integer) references users(id)</t>
+  </si>
+  <si>
+    <t>host_id (primary serial key)</t>
   </si>
 </sst>
 </file>
@@ -88,7 +100,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -101,6 +113,108 @@
       <right/>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -109,19 +223,52 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -437,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD11C8F-394E-4C94-96C6-E2D55A1B19EA}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,104 +595,172 @@
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
     <col min="6" max="6" width="11.21875" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="5"/>
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="H2" s="13"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" s="12" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="G3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="7">
         <v>7483279</v>
       </c>
-      <c r="D4" s="1">
+      <c r="C4" s="3"/>
+      <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="F4" s="3"/>
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="8">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="9">
         <v>3217848</v>
       </c>
-      <c r="D5" s="1">
+      <c r="C5" s="3"/>
+      <c r="D5" s="6">
         <v>1</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D6" s="1">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="6">
         <v>1</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D7" s="1">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D8" s="1">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="6">
         <v>2</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D9" s="1">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="8">
         <v>2</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="9" t="s">
         <v>2</v>
       </c>
-    </row>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>